<commit_message>
error handling for missing sheets in xlsx file
</commit_message>
<xml_diff>
--- a/Xlsx_Template_Prototype/CollectionX.xlsx
+++ b/Xlsx_Template_Prototype/CollectionX.xlsx
@@ -5,21 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Descriptive Metadata" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Type Of Resource Values" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Source and Location Values" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Mappings" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Mappings" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Xsls" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="departments" vbProcedure="false">'Source and Location Values'!$E$2:$E$11</definedName>
-    <definedName function="false" hidden="false" name="locations" vbProcedure="false">'Source and Location Values'!$C$2:$C$21</definedName>
-    <definedName function="false" hidden="false" name="oclcsymbol" vbProcedure="false">'Source and Location Values'!$B$2:$B$18</definedName>
-    <definedName function="false" hidden="false" name="repository" vbProcedure="false">'Source and Location Values'!$A$2:$A$22</definedName>
-    <definedName function="false" hidden="false" name="TypeOfResource" vbProcedure="false">'Type Of Resource Values'!$A$2:$A$12</definedName>
-    <definedName function="false" hidden="false" name="urls" vbProcedure="false">'Source and Location Values'!$D$2:$D$21</definedName>
+    <definedName function="false" hidden="false" name="departments" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="locations" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="oclcsymbol" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="repository" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="TypeOfResource" vbProcedure="false">#REF!</definedName>
+    <definedName function="false" hidden="false" name="urls" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="274">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -699,372 +698,6 @@
     <t xml:space="preserve">1215 x 2691</t>
   </si>
   <si>
-    <t xml:space="preserve">Guide book of New Orleans (complete work)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State Hotel Clerks Association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Orleans (La.); Vieux CarrÃ© (New Orleans, La.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete contents of a guidebook from the Louisiana State Hotel Clerks Association</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On cover: Charter 32.....Greeters of America. Week on Sunday Mar. 12, 1916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allowable Type Of Resource Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definition from LOC MODS User Guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resources that are basically textual in nature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cartographic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes maps, atlases, globes, digital maps, and other cartographic items.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notated music</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graphic, non-realized representations of musical works, both in printed and digitized manifestations that represent the four components of musical sound: pitch, duration, timbre, and loudness.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sound recording</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used when a mixture of musical and nonmusical sound recordings occurs in a resource or when a user does not want to or cannot make a distinction between musical and nonmusical.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sound recording-musical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used when a resource is predominately a musical sound recording.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sound recording-nonmusical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Used when the sound recording is nonmusical in nature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">still image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes two-dimensional images and slides and transparencies.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">moving image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes motion pictures and videorecordings, as well as television programs, digital video, and animated computer graphics—but not slides and transparencies. It does not include moving images that are primarily computer programs, such as computer games or computer-oriented multimedia; these are included in "software, multimedia".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">three dimensional object</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes man-made objects such as models, sculptures, clothing, and toys, as well as naturally occurring objects such as specimens mounted for viewing.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">software, multimedia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appropriate for any electronic resource without a significant aspect that indicates one of the other &lt;typeOfResource&gt; categories. It includes: software, numeric data, computer-oriented multimedia, and online systems and services.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mixed material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicates that there are significant materials in two or more forms that are usually related by virtue of their having been accumulated by or about a person or body. Mixed material includes archival fonds and manuscript collections of mixed forms of materials, such as text, photographs, and sound recordings.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established Source Values (A-Z)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established OCLC Member Symbol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established Physical Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established Institution Web Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Established Department</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cartographic Information Center, Department of Geography &amp;amp; Anthropology, College of Humanities and Social Sciences, Louisiana State University (http://www.cic.lsu.edu/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LHA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State Museum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://cls.louisiana.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archives and Special Collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Center for Louisiana Studies ( http://cls.louisiana.edu/ )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LHC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University Shreveport: Noel Memorial Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://lib.lsu.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archives Department</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State Museum ( http://lsm.crt.state.la.us/ )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LLM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University: Cartographic Information Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://lib.sh.lsuhsc.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hill Memorial Library: Special Collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University Health Sciences Center-Shreveport Medical Library (http://lib.sh.lsuhsc.edu)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University: LSU Libraries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://library.louisiana.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana &amp; Special Collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University in Shreveport Noel Memorial Library Archives and Special Collections (http://www.lsus.edu/library/archives.htm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University: LSU Museum of Art, Shaw Center for the Arts, Baton Rouge, LA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://library.loyno.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McNeese Archives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University Libraries, Special Collections ( http://www.lib.lsu.edu/special )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana Tech University: Prescott Memorial Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://library.mcneese.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Collections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana State University Museum of Art (http://www.lsumoa.org/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loyola University New Orleans: Monroe Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://library.nsula.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Special Collections and Archives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisiana Tech University (http://www.latech.edu/tech/library)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSU Health New Orleans: John P. Isché Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://library.uno.edu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T. Harry Williams Center for Oral History</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loyola University New Orleans Special Collections and Archives, New Orleans, LA. http://library.loyno.edu/research/speccoll/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSU Health Shreveport: Health Sciences Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ogdenmuseum.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cammie G Henry Research Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSU Health Sciences Center New Orleans ( http://www.lsuhsc.edu/library/ )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LRT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McNeese State University: Frazar Memorial Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://ulm.edu/library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Williams Research Center</t>
-  </si>
-  <si>
-    <t xml:space="preserve">McNeese State University (http://libguides.mcneese.edu/archives)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicholls State University: Ellender Memorial Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.cic.lsu.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicholls State University (http://www.nicholls.edu/library)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northwestern State University of Louisiana: University Libraries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.crt.state.la.us/louisiana-state-museum/index</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northwestern State University of Louisiana ( http://library.nsula.edu/ )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern University: John B Cade Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.hnoc.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ogden Museum of Southern Art, http://www.ogdenmuseum.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Library of Louisiana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.latech.edu/library/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Southern University, John B Cade Library, Archives Department ( http://www.lib.subr.edu/ )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LWA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Historic New Orleans Collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.lib.subr.edu/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Library of Louisiana (http://www.state.lib.la.us)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOLOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of Louisiana at Lafayette: Center for Louisiana Studies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.lsuhsc.edu/library/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T. Harry Williams Center for Oral History, a division of Louisiana State University Libraries Special Collections (http://www.lib.lsu.edu/oralhistory)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOLSM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of Louisiana at Lafayette: University Libraries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.lsumoa.org/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Historic New Orleans Collection (http://www.hnoc.org)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of Louisiana Monroe: ULM Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.lsus.edu/offices-and-services/noel-memorial-library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of Louisiana at Lafayette (http://library.louisiana.edu/)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of New Orleans: Earl K Long Library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.nicholls.edu/library</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of Louisiana at Monroe Library (http://ulm.edu/library)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of New Orleans: Ogden Museum of Southern Art</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.state.lib.la.us/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">University of New Orleans (http://library.uno.edu)</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;titleInfo&gt;&lt;title&gt;%value%&lt;/title&gt;&lt;/titleInfo&gt;</t>
   </si>
   <si>
@@ -1195,6 +828,30 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;extension&gt;&lt;hardwareSoftware&gt;%value%&lt;/hardwareSoftware&gt;&lt;/extension&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">titleNonSort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiNamePart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blankNamePart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateCreatedSplit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subjectSplit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normalizeDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OrderedTemplates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blankNodes</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +937,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1305,26 +962,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1342,12 +979,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4130,70 +3767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>222</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="J35" s="2" t="n">
-        <v>39771</v>
-      </c>
-      <c r="L35" s="0"/>
-      <c r="M35" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="O35" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="P35" s="2" t="n">
-        <v>5916</v>
-      </c>
-      <c r="Q35" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="R35" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="S35" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="U35" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="W35" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="X35" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF35" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG35" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ35" s="2" t="n">
-        <v>39771</v>
-      </c>
-      <c r="AK35" s="2" t="n">
-        <v>39790</v>
-      </c>
-      <c r="AL35" s="0" t="s">
-        <v>61</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="true" error="Please select from the list of authorized terms." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S1" type="list">
@@ -4236,491 +3810,6 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="193.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>231</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>241</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>245</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>247</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E22"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="70.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.53"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>306</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>308</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>332</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>337</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -4738,15 +3827,15 @@
         <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>344</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>345</v>
+        <v>223</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>346</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4754,7 +3843,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>347</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4762,7 +3851,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>348</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4770,7 +3859,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>349</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4778,7 +3867,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>350</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +3875,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>351</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4794,7 +3883,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>352</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4802,7 +3891,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>353</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4810,7 +3899,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>354</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4818,7 +3907,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>355</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4826,7 +3915,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>356</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4834,7 +3923,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>357</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,7 +3931,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>358</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4850,7 +3939,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>359</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4858,7 +3947,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>360</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4866,7 +3955,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>361</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4874,7 +3963,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>362</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4882,7 +3971,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>363</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4890,7 +3979,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>364</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4898,7 +3987,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>365</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,7 +3995,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>366</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4914,7 +4003,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>367</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4922,7 +4011,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>368</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4930,7 +4019,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>369</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4938,7 +4027,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>370</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4946,7 +4035,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>371</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,15 +4043,15 @@
         <v>31</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>372</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>373</v>
+        <v>251</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>374</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4970,7 +4059,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>375</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4978,7 +4067,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>376</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4986,7 +4075,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>377</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4994,7 +4083,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>378</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5002,7 +4091,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>379</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5010,7 +4099,7 @@
         <v>38</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>380</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5018,7 +4107,7 @@
         <v>39</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>381</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5026,7 +4115,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>382</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,7 +4123,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>383</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5042,7 +4131,7 @@
         <v>42</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>384</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +4139,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>385</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,7 +4147,7 @@
         <v>44</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>386</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5066,7 +4155,74 @@
         <v>45</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>387</v>
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
post processing matches expected workflow
</commit_message>
<xml_diff>
--- a/Xlsx_Template_Prototype/CollectionX.xlsx
+++ b/Xlsx_Template_Prototype/CollectionX.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="290">
   <si>
     <t xml:space="preserve">Identifier</t>
   </si>
@@ -170,13 +170,13 @@
     <t xml:space="preserve">Hardware/Software (Archival)</t>
   </si>
   <si>
-    <t xml:space="preserve">some_directory</t>
+    <t xml:space="preserve">Xlsx_Template_Prototype/CollectionX/some_directory</t>
   </si>
   <si>
     <t xml:space="preserve">as010001.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">The Picayune's little guide to New Orleans 1902</t>
+    <t xml:space="preserve">0 The Picayune's little guide to New Orleans 1902</t>
   </si>
   <si>
     <t xml:space="preserve">Stanonis, Anthony J. (Anthony Joseph)</t>
@@ -242,13 +242,13 @@
     <t xml:space="preserve">Hardware: Epson Expression 10000XL Color Flatbed Scanner Photo Model; Software: Adobe Photoshop Elements 3.0</t>
   </si>
   <si>
-    <t xml:space="preserve">another_directory</t>
+    <t xml:space="preserve">Xlsx_Template_Prototype/CollectionX/another_directory</t>
   </si>
   <si>
     <t xml:space="preserve">as010003.jp2</t>
   </si>
   <si>
-    <t xml:space="preserve">Tourist's guide to New Orleans</t>
+    <t xml:space="preserve">1 Tourist's guide to New Orleans</t>
   </si>
   <si>
     <t xml:space="preserve">Times-Picayune Pub. Co.</t>
@@ -266,13 +266,13 @@
     <t xml:space="preserve">14,181 KB</t>
   </si>
   <si>
-    <t xml:space="preserve">another_directory/subdirectory</t>
+    <t xml:space="preserve">Xlsx_Template_Prototype/CollectionX/another_directory/subdirectory</t>
   </si>
   <si>
     <t xml:space="preserve">as010007.jp2</t>
   </si>
   <si>
-    <t xml:space="preserve">Vieux Carré Guide</t>
+    <t xml:space="preserve">2 Vieux Carre Guide</t>
   </si>
   <si>
     <t xml:space="preserve">Cover image of a New Orleans guidebook</t>
@@ -290,7 +290,7 @@
     <t xml:space="preserve">as010014.jp2</t>
   </si>
   <si>
-    <t xml:space="preserve">The Louisiana tourist, Vol. 1 - No. 1</t>
+    <t xml:space="preserve">3 The Louisiana tourist, Vol. 1 - No. 1</t>
   </si>
   <si>
     <t xml:space="preserve">Louisiana Department of Commerce and Industry, Tourism Bureau</t>
@@ -299,7 +299,7 @@
     <t xml:space="preserve">Louisiana -- Guidebooks; Louisiana -- Description and travel; Louisiana -- Tours</t>
   </si>
   <si>
-    <t xml:space="preserve">New Orleans (La.); Vieux Carré (New Orleans, La.)</t>
+    <t xml:space="preserve">New Orleans (La.); Vieux Carre (New Orleans, La.)</t>
   </si>
   <si>
     <t xml:space="preserve">1938-11</t>
@@ -320,7 +320,7 @@
     <t xml:space="preserve">as010008.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">New Orleans: America's second port. The south's greatest industrial city</t>
+    <t xml:space="preserve">4 New Orleans: America's second port. The south's greatest industrial city</t>
   </si>
   <si>
     <t xml:space="preserve">Cover image of a New Orleans guidebook.</t>
@@ -338,7 +338,7 @@
     <t xml:space="preserve">as010012.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Souvenir harbor guide: New Orleans second port U.S.A.</t>
+    <t xml:space="preserve">5 Souvenir harbor guide: New Orleans second port U.S.A.</t>
   </si>
   <si>
     <t xml:space="preserve">Streckfus Steamers, Inc.</t>
@@ -359,7 +359,7 @@
     <t xml:space="preserve">as010015.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Historic old New Orleans: America's most interesting city</t>
+    <t xml:space="preserve">6 Historic old New Orleans: America's most interesting city</t>
   </si>
   <si>
     <t xml:space="preserve">On cover: Courtyard, Governor Claiborne Home; Complete guidebook available in collection 21, series 1, folder 15</t>
@@ -374,7 +374,7 @@
     <t xml:space="preserve">as010018.jp2</t>
   </si>
   <si>
-    <t xml:space="preserve">Guide to New Orleans and environs. Sixth edition</t>
+    <t xml:space="preserve">7 Guide to New Orleans and environs. Sixth edition</t>
   </si>
   <si>
     <t xml:space="preserve">Bremer, Laville</t>
@@ -395,7 +395,7 @@
     <t xml:space="preserve">as010023.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">1952 visitors guide: what to see in and around New Orleans</t>
+    <t xml:space="preserve">8 1952 visitors guide: what to see in and around New Orleans</t>
   </si>
   <si>
     <t xml:space="preserve">New Orleans Item</t>
@@ -413,7 +413,7 @@
     <t xml:space="preserve">as010026.jp2</t>
   </si>
   <si>
-    <t xml:space="preserve">This week in New Orleans, Vol. 60 - No. 2</t>
+    <t xml:space="preserve">9 This week in New Orleans, Vol. 60 - No. 2</t>
   </si>
   <si>
     <t xml:space="preserve">On cover: Helen Re[ed], Enjoy New Orleans and Mississippi's Coast; Complete guidebook available in collection 21, series 1, folder 26</t>
@@ -425,10 +425,31 @@
     <t xml:space="preserve">10914 KB</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Xlsx_Template_Prototype/CollectionX/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">another_directory</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">as010031.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Fascinating New Orleans as seen with Southern Tours</t>
+    <t xml:space="preserve">10 Fascinating New Orleans as seen with Southern Tours</t>
   </si>
   <si>
     <t xml:space="preserve">Southern Tours Inc.</t>
@@ -443,7 +464,7 @@
     <t xml:space="preserve">as020003.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Original Cookes tour of the city: the right way to see New Orleans</t>
+    <t xml:space="preserve">11 Original Cookes tour of the city: the right way to see New Orleans</t>
   </si>
   <si>
     <t xml:space="preserve">On cover: Phone M. 49 or M. 50, Fare $1.00 Trip.; Complete guidebook available in collection 21, series 2, folder 3</t>
@@ -458,7 +479,7 @@
     <t xml:space="preserve">as020011.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">A little guide to New Orleans for soldiers, sailors, marines</t>
+    <t xml:space="preserve">12 A little guide to New Orleans for soldiers, sailors, marines</t>
   </si>
   <si>
     <t xml:space="preserve">New Orleans War Camp Community Service</t>
@@ -479,7 +500,7 @@
     <t xml:space="preserve">as020014.jp2</t>
   </si>
   <si>
-    <t xml:space="preserve">New Orleans nonsense</t>
+    <t xml:space="preserve">13 New Orleans nonsense</t>
   </si>
   <si>
     <t xml:space="preserve">Vernon, Arthur</t>
@@ -500,7 +521,7 @@
     <t xml:space="preserve">as020016.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">The New Orleans visitor's guide</t>
+    <t xml:space="preserve">14 The New Orleans visitor's guide</t>
   </si>
   <si>
     <t xml:space="preserve">On covere: Free-take one. Visitors City Guide. Free-take one; Complete guidebook available in collection 21, series 2, folder 16</t>
@@ -515,7 +536,7 @@
     <t xml:space="preserve">as020020.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Seeing New Orleans with Royal Sightseeing</t>
+    <t xml:space="preserve">15 Seeing New Orleans with Royal Sightseeing</t>
   </si>
   <si>
     <t xml:space="preserve">Royal Tours Inc.</t>
@@ -536,7 +557,7 @@
     <t xml:space="preserve">as020027.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">World's longest bridge</t>
+    <t xml:space="preserve">16 World's longest bridge</t>
   </si>
   <si>
     <t xml:space="preserve">New Orleans (La.) -- Description and travel; New Orleans (La.) -- Guidebooks; New Orleans (La.) -- Tours; Lake Pontchartrain Causeway</t>
@@ -557,7 +578,7 @@
     <t xml:space="preserve">as020008.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Historic -- Old New Orleans, La.</t>
+    <t xml:space="preserve">17 Historic -- Old New Orleans, La.</t>
   </si>
   <si>
     <t xml:space="preserve">On cover: Ancient Driveway. French Quarter; Complete guidebook available in collection 21, series 2, folder 8</t>
@@ -572,7 +593,7 @@
     <t xml:space="preserve">as020024.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Visitor's guide to New Orleans: Seeing New Orleans the unique water way</t>
+    <t xml:space="preserve">18Visitor's guide to New Orleans: Seeing New Orleans the unique water way</t>
   </si>
   <si>
     <t xml:space="preserve">On cover: Free map-take one. 21/2 hour sight-seeing and pleasure tour on Mark Twain's historic Mississippi River, Daily Trips Leave 2:30 pm - Return 5:00 pm, A Delightful Ride on a Big Mississippi River Steamer; Complete guidebook available in collection 21, series 2, folder 24</t>
@@ -584,13 +605,19 @@
     <t xml:space="preserve">8,116 KB</t>
   </si>
   <si>
+    <t xml:space="preserve">19 0 A Compound Item</t>
+  </si>
+  <si>
     <t xml:space="preserve">01</t>
   </si>
   <si>
+    <t xml:space="preserve">Xlsx_Template_Prototype/CollectionX/33</t>
+  </si>
+  <si>
     <t xml:space="preserve">as010004_0001.tif</t>
   </si>
   <si>
-    <t xml:space="preserve">Guide Book of New Orleans</t>
+    <t xml:space="preserve">19 01 Guide Book of New Orleans</t>
   </si>
   <si>
     <t xml:space="preserve">1209 x 2703</t>
@@ -605,6 +632,9 @@
     <t xml:space="preserve">as010004_0002.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 02Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">2441 x 2732</t>
   </si>
   <si>
@@ -617,12 +647,18 @@
     <t xml:space="preserve">as010004_0003.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 03 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">04</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0004.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 04 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">19,567 KB</t>
   </si>
   <si>
@@ -632,30 +668,45 @@
     <t xml:space="preserve">as010004_0005.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 05 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">06</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0006.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 06 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">07</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0007.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 07 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">08</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0008.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 08 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">09</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0009.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 09 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">2417 x 2708</t>
   </si>
   <si>
@@ -668,6 +719,9 @@
     <t xml:space="preserve">as010004_0010.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 10 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">19,204 KB</t>
   </si>
   <si>
@@ -677,22 +731,34 @@
     <t xml:space="preserve">as010004_0011.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 11 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">12</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0012.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 12 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">13</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0013.jp2</t>
   </si>
   <si>
+    <t xml:space="preserve">19 13 Guide Book of New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">as010004_0014.tif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19 14 Guide Book of New Orleans</t>
   </si>
   <si>
     <t xml:space="preserve">1215 x 2691</t>
@@ -863,7 +929,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -893,6 +959,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -937,7 +1009,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -962,6 +1034,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -979,18 +1055,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="0" width="10.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.9"/>
@@ -2107,25 +2183,25 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="0" t="s">
-        <v>70</v>
+      <c r="C12" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>49</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J12" s="2" t="n">
         <v>39769</v>
@@ -2143,10 +2219,10 @@
         <v>1960</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="S12" s="0" t="s">
         <v>55</v>
@@ -2203,10 +2279,10 @@
         <v>70</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>49</v>
@@ -2227,7 +2303,7 @@
         <v>97</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="S13" s="0" t="s">
         <v>55</v>
@@ -2269,13 +2345,13 @@
         <v>65</v>
       </c>
       <c r="AQ13" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AR13" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS13" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AT13" s="0" t="s">
         <v>69</v>
@@ -2290,16 +2366,16 @@
         <v>70</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>49</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J14" s="2" t="n">
         <v>39769</v>
@@ -2314,10 +2390,10 @@
         <v>89</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="S14" s="0" t="s">
         <v>55</v>
@@ -2359,13 +2435,13 @@
         <v>65</v>
       </c>
       <c r="AQ14" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AR14" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS14" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AT14" s="0" t="s">
         <v>69</v>
@@ -2380,13 +2456,13 @@
         <v>70</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>49</v>
@@ -2404,10 +2480,10 @@
         <v>89</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="S15" s="0" t="s">
         <v>55</v>
@@ -2449,13 +2525,13 @@
         <v>65</v>
       </c>
       <c r="AQ15" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AR15" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS15" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AT15" s="0" t="s">
         <v>69</v>
@@ -2470,10 +2546,10 @@
         <v>46</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>49</v>
@@ -2494,7 +2570,7 @@
         <v>97</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="S16" s="0" t="s">
         <v>55</v>
@@ -2536,13 +2612,13 @@
         <v>65</v>
       </c>
       <c r="AQ16" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AR16" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS16" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AT16" s="0" t="s">
         <v>69</v>
@@ -2557,16 +2633,16 @@
         <v>46</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>49</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J17" s="2" t="n">
         <v>39769</v>
@@ -2581,10 +2657,10 @@
         <v>89</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="S17" s="0" t="s">
         <v>55</v>
@@ -2626,13 +2702,13 @@
         <v>65</v>
       </c>
       <c r="AQ17" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AR17" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS17" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AT17" s="0" t="s">
         <v>69</v>
@@ -2647,10 +2723,10 @@
         <v>46</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>49</v>
@@ -2662,16 +2738,16 @@
         <v>39407</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q18" s="0" t="s">
         <v>97</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="S18" s="0" t="s">
         <v>55</v>
@@ -2713,13 +2789,13 @@
         <v>65</v>
       </c>
       <c r="AQ18" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AR18" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS18" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AT18" s="0" t="s">
         <v>69</v>
@@ -2734,10 +2810,10 @@
         <v>46</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>49</v>
@@ -2758,7 +2834,7 @@
         <v>97</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="S19" s="0" t="s">
         <v>55</v>
@@ -2800,13 +2876,13 @@
         <v>65</v>
       </c>
       <c r="AQ19" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="AR19" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS19" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AT19" s="0" t="s">
         <v>69</v>
@@ -2821,10 +2897,10 @@
         <v>46</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>49</v>
@@ -2839,13 +2915,13 @@
         <v>51</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q20" s="0" t="s">
         <v>97</v>
       </c>
       <c r="R20" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="S20" s="0" t="s">
         <v>55</v>
@@ -2887,13 +2963,13 @@
         <v>65</v>
       </c>
       <c r="AQ20" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AR20" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS20" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AT20" s="0" t="s">
         <v>69</v>
@@ -2903,17 +2979,9 @@
       <c r="A21" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C21" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="B21" s="1"/>
+      <c r="E21" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>186</v>
       </c>
       <c r="J21" s="2" t="n">
         <v>39771</v>
@@ -2921,61 +2989,19 @@
       <c r="L21" s="2" t="n">
         <v>39407</v>
       </c>
-      <c r="X21" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG21" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ21" s="2" t="n">
-        <v>39771</v>
-      </c>
-      <c r="AK21" s="2" t="n">
-        <v>39771</v>
-      </c>
-      <c r="AL21" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AM21" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN21" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AO21" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AP21" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ21" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="AR21" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AS21" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="AT21" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="E22" s="0" t="s">
         <v>189</v>
-      </c>
-      <c r="C22" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>186</v>
       </c>
       <c r="J22" s="2" t="n">
         <v>39771</v>
@@ -3011,33 +3037,30 @@
         <v>65</v>
       </c>
       <c r="AQ22" s="0" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AR22" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS22" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AT22" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>21</v>
-      </c>
       <c r="B23" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="C23" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>194</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>186</v>
       </c>
       <c r="J23" s="2" t="n">
         <v>39771</v>
@@ -3073,33 +3096,30 @@
         <v>65</v>
       </c>
       <c r="AQ23" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AR23" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS23" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="AT23" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>22</v>
-      </c>
       <c r="B24" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>33</v>
+        <v>197</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="J24" s="2" t="n">
         <v>39771</v>
@@ -3135,33 +3155,30 @@
         <v>65</v>
       </c>
       <c r="AQ24" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AR24" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS24" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AT24" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>23</v>
-      </c>
       <c r="B25" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C25" s="0" t="n">
-        <v>33</v>
+        <v>200</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="J25" s="2" t="n">
         <v>39771</v>
@@ -3197,33 +3214,30 @@
         <v>65</v>
       </c>
       <c r="AQ25" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AR25" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS25" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="AT25" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>24</v>
-      </c>
       <c r="B26" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>33</v>
+        <v>204</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="J26" s="2" t="n">
         <v>39771</v>
@@ -3259,33 +3273,30 @@
         <v>65</v>
       </c>
       <c r="AQ26" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AR26" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS26" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="AT26" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>25</v>
-      </c>
       <c r="B27" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>33</v>
+        <v>207</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="J27" s="2" t="n">
         <v>39771</v>
@@ -3321,33 +3332,30 @@
         <v>65</v>
       </c>
       <c r="AQ27" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AR27" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS27" s="0" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AT27" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>26</v>
-      </c>
       <c r="B28" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>33</v>
+        <v>210</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="J28" s="2" t="n">
         <v>39771</v>
@@ -3383,33 +3391,30 @@
         <v>65</v>
       </c>
       <c r="AQ28" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="AR28" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS28" s="0" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="AT28" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>27</v>
-      </c>
       <c r="B29" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C29" s="0" t="n">
-        <v>33</v>
+        <v>213</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="J29" s="2" t="n">
         <v>39771</v>
@@ -3445,33 +3450,30 @@
         <v>65</v>
       </c>
       <c r="AQ29" s="0" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="AR29" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS29" s="0" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="AT29" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="B30" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <v>33</v>
+        <v>216</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="J30" s="2" t="n">
         <v>39771</v>
@@ -3507,33 +3509,30 @@
         <v>65</v>
       </c>
       <c r="AQ30" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="AR30" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS30" s="0" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="AT30" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>29</v>
-      </c>
       <c r="B31" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C31" s="0" t="n">
-        <v>33</v>
+        <v>221</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="J31" s="2" t="n">
         <v>39771</v>
@@ -3569,33 +3568,30 @@
         <v>65</v>
       </c>
       <c r="AQ31" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="AR31" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS31" s="0" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="AT31" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>30</v>
-      </c>
       <c r="B32" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>33</v>
+        <v>225</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>186</v>
+        <v>227</v>
       </c>
       <c r="J32" s="2" t="n">
         <v>39771</v>
@@ -3631,33 +3627,30 @@
         <v>65</v>
       </c>
       <c r="AQ32" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="AR32" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS32" s="0" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="AT32" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>31</v>
-      </c>
       <c r="B33" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C33" s="0" t="n">
-        <v>33</v>
+        <v>228</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>186</v>
+        <v>230</v>
       </c>
       <c r="J33" s="2" t="n">
         <v>39771</v>
@@ -3693,33 +3686,30 @@
         <v>65</v>
       </c>
       <c r="AQ33" s="0" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="AR33" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS33" s="0" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="AT33" s="0" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>32</v>
-      </c>
       <c r="B34" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C34" s="0" t="n">
-        <v>33</v>
+        <v>231</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>187</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>186</v>
+        <v>233</v>
       </c>
       <c r="J34" s="2" t="n">
         <v>39771</v>
@@ -3755,19 +3745,77 @@
         <v>65</v>
       </c>
       <c r="AQ34" s="0" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AR34" s="0" t="s">
         <v>67</v>
       </c>
       <c r="AS34" s="0" t="s">
-        <v>166</v>
+        <v>224</v>
       </c>
       <c r="AT34" s="0" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>39771</v>
+      </c>
+      <c r="L35" s="2" t="n">
+        <v>39407</v>
+      </c>
+      <c r="X35" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG35" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ35" s="2" t="n">
+        <v>39771</v>
+      </c>
+      <c r="AK35" s="2" t="n">
+        <v>39771</v>
+      </c>
+      <c r="AL35" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AM35" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN35" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO35" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP35" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ35" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="AR35" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS35" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="AT35" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="6">
     <dataValidation allowBlank="true" error="Please select from the list of authorized terms." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S1" type="list">
@@ -3812,7 +3860,7 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -3827,15 +3875,15 @@
         <v>4</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3843,7 +3891,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,7 +3899,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3859,7 +3907,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3867,7 +3915,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3875,7 +3923,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3883,7 +3931,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3891,7 +3939,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3899,7 +3947,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3907,7 +3955,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3915,7 +3963,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3923,7 +3971,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,7 +3979,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3939,7 +3987,7 @@
         <v>18</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3947,7 +3995,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3955,7 +4003,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3963,7 +4011,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3971,7 +4019,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3979,7 +4027,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3987,7 +4035,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3995,7 +4043,7 @@
         <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4003,7 +4051,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4011,7 +4059,7 @@
         <v>27</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4019,7 +4067,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4027,7 +4075,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4035,7 +4083,7 @@
         <v>30</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4043,15 +4091,15 @@
         <v>31</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4059,7 +4107,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4067,7 +4115,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4075,7 +4123,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4083,7 +4131,7 @@
         <v>36</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,7 +4139,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4099,7 +4147,7 @@
         <v>38</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4107,7 +4155,7 @@
         <v>39</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4115,7 +4163,7 @@
         <v>40</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4123,7 +4171,7 @@
         <v>41</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,7 +4179,7 @@
         <v>42</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4139,7 +4187,7 @@
         <v>43</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4147,7 +4195,7 @@
         <v>44</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4155,7 +4203,7 @@
         <v>45</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4176,7 +4224,7 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4187,42 +4235,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>